<commit_message>
PRF ACK and Template PRF ACK
</commit_message>
<xml_diff>
--- a/Template_PRF.xlsx
+++ b/Template_PRF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Python\excelProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8575BDFC-18BF-47BA-84CD-64A286B9299D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C33B467-52ED-470B-B19E-B654C3F55969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRF" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>G(13)-1687732</t>
   </si>
@@ -54,9 +54,6 @@
     <t>WHEREAS THE ABOVE-NAMED PRINCIPAL WAS AWARDED AND GUARANTEES THE FAITHFUL PERFORMANCE FOR THE PROJECT:</t>
   </si>
   <si>
-    <t>PUBLICATION OF ORDINANCES</t>
-  </si>
-  <si>
     <t>The Performance security shall remain valid until issuance by the procuring entity the final certificate of acceptance.</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>PROVIDED HOWEVER, that the maximum limit of the surety hereunder shall in no case exceed the sum of PESOS:</t>
   </si>
   <si>
-    <t>ONE HUNDRED FORTY NINE THOUSAND FOUR HUNDRED TEN  PESOS ONLY</t>
-  </si>
-  <si>
-    <t>(Php149,410.00; Philippine Currencies)</t>
-  </si>
-  <si>
     <t>CONTRACT</t>
   </si>
   <si>
@@ -102,12 +93,6 @@
     <t>Legazpi City</t>
   </si>
   <si>
-    <t>*January 11, 2023</t>
-  </si>
-  <si>
-    <t>ONE HUNDRED FORTY NINE THOUSAND</t>
-  </si>
-  <si>
     <t>FOUR HUNDRED TEN  PESOS ONLY</t>
   </si>
   <si>
@@ -126,21 +111,9 @@
     <t>BICOL PERYODIKO</t>
   </si>
   <si>
-    <t>JULY 29, 2026</t>
-  </si>
-  <si>
     <t>JULY 29, 2025</t>
   </si>
   <si>
-    <t xml:space="preserve">                             STEPHANIE M. RAMIREZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STEPHANIE M. RAMIREZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STEPHANIE M. RAMIREZ - BRANCH MANAGER</t>
-  </si>
-  <si>
     <t xml:space="preserve">JULY 29, 2025 </t>
   </si>
   <si>
@@ -156,12 +129,6 @@
     <t>TWO THOUSAND THREE  HUNDRED FIFTY</t>
   </si>
   <si>
-    <t>January 9, 2025</t>
-  </si>
-  <si>
-    <t>Cavinitan , Virac, Catanduanes</t>
-  </si>
-  <si>
     <t xml:space="preserve">BOND NO. </t>
   </si>
   <si>
@@ -175,6 +142,63 @@
   </si>
   <si>
     <t xml:space="preserve">AMOUNT IN WORDS </t>
+  </si>
+  <si>
+    <t>CONTRACT NAME</t>
+  </si>
+  <si>
+    <t>AMOUNT IN WORDS</t>
+  </si>
+  <si>
+    <t>(PhpCOVERAGE; Philippine Currencies)</t>
+  </si>
+  <si>
+    <t>DATE, YEAR + 1</t>
+  </si>
+  <si>
+    <t>DATE, YEAR</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t>PROPRIETOR</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>BOND NO.</t>
+  </si>
+  <si>
+    <t>CTC</t>
+  </si>
+  <si>
+    <t>CTC DATE</t>
+  </si>
+  <si>
+    <t>CTC MANAGER DATE</t>
+  </si>
+  <si>
+    <t>CTC MANAGER</t>
+  </si>
+  <si>
+    <t>DATE, 2025</t>
+  </si>
+  <si>
+    <t>MANAGER - BRANCH MANAGER</t>
+  </si>
+  <si>
+    <t>AMOUNT IN WORDS 1</t>
+  </si>
+  <si>
+    <t>AMOUNT IN WORDS 2</t>
+  </si>
+  <si>
+    <t>COVERAGE</t>
+  </si>
+  <si>
+    <t>PROP ADD</t>
   </si>
 </sst>
 </file>
@@ -390,9 +414,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,6 +448,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -770,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +918,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="36" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K10" s="37"/>
     </row>
@@ -968,13 +992,13 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="36" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="25" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="K16" s="10"/>
     </row>
@@ -1035,19 +1059,21 @@
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="H21" s="25" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="9" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="8"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="J22" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1137,7 +1163,7 @@
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="9" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1147,43 +1173,43 @@
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="9" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="9" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,7 +1232,7 @@
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -1322,7 +1348,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="10"/>
       <c r="C49" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
@@ -1396,7 +1422,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K54" s="10"/>
     </row>
@@ -1418,11 +1444,11 @@
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
@@ -1523,16 +1549,16 @@
     </row>
     <row r="64" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
-      <c r="B64" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
+      <c r="B64" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="52"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="52"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="36" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I64" s="36"/>
       <c r="J64" s="36"/>
@@ -1593,7 +1619,7 @@
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
@@ -1674,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1743,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="36" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K3" s="37"/>
     </row>
@@ -1737,7 +1763,7 @@
     <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1770,7 +1796,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -1821,16 +1847,16 @@
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="42">
-        <v>140835</v>
-      </c>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="42"/>
       <c r="G11" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J11" s="23"/>
       <c r="K11" s="14"/>
@@ -1849,31 +1875,34 @@
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="E13" s="39">
-        <v>1993932</v>
-      </c>
-      <c r="F13" s="39"/>
+      <c r="B13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="38"/>
       <c r="G13" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="21" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
-      <c r="B14" s="14" t="s">
-        <v>32</v>
+      <c r="B14" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -1882,9 +1911,6 @@
     </row>
     <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="20" t="s">
-        <v>16</v>
-      </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -1990,7 +2016,7 @@
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -2160,7 +2186,7 @@
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
@@ -2189,7 +2215,7 @@
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -2265,15 +2291,15 @@
       <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="41" t="s">
-        <v>22</v>
+      <c r="A44" s="40" t="s">
+        <v>50</v>
       </c>
       <c r="B44" s="37"/>
       <c r="C44" s="37"/>
       <c r="D44" s="37"/>
       <c r="E44" s="37"/>
-      <c r="F44" s="45">
-        <v>149410</v>
+      <c r="F44" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="G44" s="37"/>
       <c r="H44" s="37"/>
@@ -2281,14 +2307,14 @@
       <c r="K44" s="14"/>
     </row>
     <row r="45" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
-        <v>23</v>
+      <c r="A45" s="40" t="s">
+        <v>51</v>
       </c>
       <c r="B45" s="37"/>
       <c r="C45" s="37"/>
       <c r="D45" s="37"/>
       <c r="E45" s="37"/>
-      <c r="F45" s="44"/>
+      <c r="F45" s="43"/>
       <c r="G45" s="37"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
@@ -2342,11 +2368,11 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
-      <c r="H49" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41"/>
+      <c r="H49" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
       <c r="K49" s="14"/>
     </row>
     <row r="50" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2410,7 +2436,7 @@
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
       <c r="H54" s="9" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -2426,8 +2452,8 @@
       <c r="G55" s="11"/>
       <c r="H55" s="19"/>
       <c r="I55" s="11"/>
-      <c r="J55" s="39">
-        <v>11070531</v>
+      <c r="J55" s="38" t="s">
+        <v>47</v>
       </c>
       <c r="K55" s="37"/>
     </row>
@@ -2440,7 +2466,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="15" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="I56" s="15"/>
       <c r="J56" s="19"/>
@@ -2460,8 +2486,8 @@
     </row>
     <row r="58" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
-      <c r="B58" s="40" t="s">
-        <v>15</v>
+      <c r="B58" s="39" t="s">
+        <v>12</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="11"/>
@@ -2885,15 +2911,15 @@
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="49" t="s">
-        <v>28</v>
+      <c r="B17" s="48" t="s">
+        <v>23</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="46" t="s">
-        <v>35</v>
+      <c r="G17" s="45" t="s">
+        <v>26</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
@@ -2902,13 +2928,13 @@
     </row>
     <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="48" t="s">
-        <v>23</v>
+      <c r="B18" s="47" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
-      <c r="F18" s="47">
+      <c r="F18" s="46">
         <v>149410</v>
       </c>
       <c r="G18" s="37"/>
@@ -2919,7 +2945,7 @@
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="47" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="37"/>
@@ -2991,8 +3017,8 @@
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="46" t="s">
-        <v>24</v>
+      <c r="G24" s="45" t="s">
+        <v>19</v>
       </c>
       <c r="H24" s="37"/>
       <c r="I24" s="37"/>
@@ -3002,12 +3028,12 @@
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="47">
+      <c r="F25" s="46">
         <v>1246.3008</v>
       </c>
       <c r="G25" s="37"/>
@@ -3024,7 +3050,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -3098,7 +3124,7 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3353,7 +3379,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -3479,7 +3505,7 @@
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -3500,7 +3526,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
@@ -3522,7 +3548,7 @@
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -3735,7 +3761,7 @@
     <row r="43" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -3769,7 +3795,7 @@
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -3882,7 +3908,7 @@
     <row r="54" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -4066,7 +4092,7 @@
     </row>
     <row r="5" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -4079,11 +4105,11 @@
     </row>
     <row r="6" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
-      <c r="B6" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="6"/>
@@ -4100,16 +4126,16 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="6"/>
@@ -4143,7 +4169,7 @@
     </row>
     <row r="12" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="30"/>
@@ -4154,7 +4180,7 @@
     <row r="13" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="10"/>
@@ -4167,8 +4193,8 @@
     </row>
     <row r="14" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="43"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -4176,10 +4202,10 @@
     </row>
     <row r="15" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -4188,7 +4214,7 @@
     <row r="16" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -4205,11 +4231,11 @@
     </row>
     <row r="18" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="31">
@@ -4221,7 +4247,7 @@
     <row r="19" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -4232,7 +4258,7 @@
       <c r="A20" s="10"/>
       <c r="B20" s="17"/>
       <c r="C20" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -4242,7 +4268,7 @@
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4252,7 +4278,7 @@
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="31">
@@ -4276,7 +4302,7 @@
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E24" s="10"/>
       <c r="G24" s="6"/>
@@ -4284,7 +4310,7 @@
     <row r="25" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="32"/>
@@ -4350,7 +4376,7 @@
       <c r="B31" s="32"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E31" s="30"/>
       <c r="F31" s="6"/>
@@ -4407,7 +4433,7 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -4421,7 +4447,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -4435,7 +4461,7 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>

</xml_diff>

<commit_message>
Finalized PRF and Template
</commit_message>
<xml_diff>
--- a/Template_PRF.xlsx
+++ b/Template_PRF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Python\excelProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C33B467-52ED-470B-B19E-B654C3F55969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A45417-2B6B-4FEE-A512-CCED5221B476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRF" sheetId="1" r:id="rId1"/>
@@ -37,19 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
-  <si>
-    <t>G(13)-1687732</t>
-  </si>
-  <si>
-    <t>bicol peryodiko</t>
-  </si>
-  <si>
-    <t>CAVINITAN, VIRAC, CATANDUANES</t>
-  </si>
-  <si>
-    <t>LGU-BARAS, CATANDUANES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>WHEREAS THE ABOVE-NAMED PRINCIPAL WAS AWARDED AND GUARANTEES THE FAITHFUL PERFORMANCE FOR THE PROJECT:</t>
   </si>
@@ -78,9 +66,6 @@
     <t/>
   </si>
   <si>
-    <t>MR. FERDINAND M. BRIZO</t>
-  </si>
-  <si>
     <t>GEMMA T. SARMIENTO</t>
   </si>
   <si>
@@ -93,42 +78,9 @@
     <t>Legazpi City</t>
   </si>
   <si>
-    <t>FOUR HUNDRED TEN  PESOS ONLY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONE THOUSAND TWO HUNDRED FORTY SIX  </t>
-  </si>
-  <si>
-    <t>AND 30/100 ONLY</t>
-  </si>
-  <si>
     <t>ONE (1) YEAR</t>
   </si>
   <si>
-    <t>FOUR  PESOS AND 14/100 ONLY</t>
-  </si>
-  <si>
-    <t>BICOL PERYODIKO</t>
-  </si>
-  <si>
-    <t>JULY 29, 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JULY 29, 2025 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONE HUNDRED FORTY NINE THOUSAND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 JULY 29, 2025 </t>
-  </si>
-  <si>
-    <t>JULY 29, 2025  - JULY 29, 2026</t>
-  </si>
-  <si>
-    <t>TWO THOUSAND THREE  HUNDRED FIFTY</t>
-  </si>
-  <si>
     <t xml:space="preserve">BOND NO. </t>
   </si>
   <si>
@@ -153,6 +105,9 @@
     <t>(PhpCOVERAGE; Philippine Currencies)</t>
   </si>
   <si>
+    <t>DATE</t>
+  </si>
+  <si>
     <t>DATE, YEAR + 1</t>
   </si>
   <si>
@@ -199,6 +154,27 @@
   </si>
   <si>
     <t>PROP ADD</t>
+  </si>
+  <si>
+    <t>AMOUNTS IN WORDS 2</t>
+  </si>
+  <si>
+    <t>RATING AMOUNT IN WORDS</t>
+  </si>
+  <si>
+    <t>RATING AMOUNT IN WORDS 2</t>
+  </si>
+  <si>
+    <t>RATING AMOUNT</t>
+  </si>
+  <si>
+    <t>PROP ADRESS</t>
+  </si>
+  <si>
+    <t>BOND NO</t>
+  </si>
+  <si>
+    <t>DATE YEAR - DATE YEAR + 1</t>
   </si>
 </sst>
 </file>
@@ -918,7 +894,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="36" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="K10" s="37"/>
     </row>
@@ -992,13 +968,13 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="36" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="25" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="K16" s="10"/>
     </row>
@@ -1059,20 +1035,20 @@
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="H21" s="25" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="9" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="8"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="K22" s="10"/>
     </row>
@@ -1157,13 +1133,13 @@
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1173,43 +1149,43 @@
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="9" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1208,7 @@
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -1348,7 +1324,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="10"/>
       <c r="C49" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
@@ -1422,7 +1398,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K54" s="10"/>
     </row>
@@ -1444,11 +1420,11 @@
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="9" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
@@ -1550,7 +1526,7 @@
     <row r="64" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="36" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C64" s="52"/>
       <c r="D64" s="52"/>
@@ -1558,7 +1534,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="36" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I64" s="36"/>
       <c r="J64" s="36"/>
@@ -1619,7 +1595,7 @@
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="25" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
@@ -1700,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,7 +1719,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="36" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="K3" s="37"/>
     </row>
@@ -1763,7 +1739,7 @@
     <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1796,7 +1772,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="9" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -1848,15 +1824,15 @@
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="41" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="J11" s="23"/>
       <c r="K11" s="14"/>
@@ -1876,18 +1852,18 @@
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="21" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="14"/>
@@ -1895,14 +1871,14 @@
     <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="20" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -2016,7 +1992,7 @@
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -2186,7 +2162,7 @@
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
@@ -2215,7 +2191,7 @@
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -2292,14 +2268,14 @@
     </row>
     <row r="44" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B44" s="37"/>
       <c r="C44" s="37"/>
       <c r="D44" s="37"/>
       <c r="E44" s="37"/>
       <c r="F44" s="44" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G44" s="37"/>
       <c r="H44" s="37"/>
@@ -2308,7 +2284,7 @@
     </row>
     <row r="45" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B45" s="37"/>
       <c r="C45" s="37"/>
@@ -2369,7 +2345,7 @@
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
       <c r="H49" s="40" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="I49" s="40"/>
       <c r="J49" s="40"/>
@@ -2436,7 +2412,7 @@
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
       <c r="H54" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -2453,7 +2429,7 @@
       <c r="H55" s="19"/>
       <c r="I55" s="11"/>
       <c r="J55" s="38" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="K55" s="37"/>
     </row>
@@ -2466,7 +2442,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="15" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I56" s="15"/>
       <c r="J56" s="19"/>
@@ -2487,7 +2463,7 @@
     <row r="58" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="11"/>
@@ -2693,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,7 +2686,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="36" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K1" s="37"/>
     </row>
@@ -2912,14 +2888,14 @@
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="48" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
       <c r="F17" s="7"/>
       <c r="G17" s="45" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
@@ -2929,13 +2905,13 @@
     <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="47" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
-      <c r="F18" s="46">
-        <v>149410</v>
+      <c r="F18" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="4"/>
@@ -2946,7 +2922,7 @@
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="47" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
@@ -3018,7 +2994,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="45" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="H24" s="37"/>
       <c r="I24" s="37"/>
@@ -3028,13 +3004,13 @@
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="10" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="46">
-        <v>1246.3008</v>
+      <c r="F25" s="46" t="s">
+        <v>42</v>
       </c>
       <c r="G25" s="37"/>
       <c r="H25" s="4"/>
@@ -3050,7 +3026,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -3124,7 +3100,7 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3194,8 +3170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,7 +3355,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -3505,7 +3481,7 @@
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -3548,14 +3524,14 @@
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="13" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="11" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -3565,7 +3541,7 @@
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -3761,7 +3737,7 @@
     <row r="43" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -3795,7 +3771,7 @@
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -3908,14 +3884,14 @@
     <row r="54" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -4028,8 +4004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4091,10 +4067,10 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="10"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4106,7 +4082,7 @@
     <row r="6" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="49" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
@@ -4127,15 +4103,15 @@
     </row>
     <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="42"/>
       <c r="D8" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="6"/>
@@ -4169,7 +4145,7 @@
     </row>
     <row r="12" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="30"/>
@@ -4180,7 +4156,7 @@
     <row r="13" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="10"/>
@@ -4203,7 +4179,7 @@
     <row r="15" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="51" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="10"/>
@@ -4214,7 +4190,7 @@
     <row r="16" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -4231,11 +4207,11 @@
     </row>
     <row r="18" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="31">
@@ -4247,7 +4223,7 @@
     <row r="19" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -4258,7 +4234,7 @@
       <c r="A20" s="10"/>
       <c r="B20" s="17"/>
       <c r="C20" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -4268,7 +4244,7 @@
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4278,7 +4254,7 @@
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="31">
@@ -4302,7 +4278,7 @@
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E24" s="10"/>
       <c r="G24" s="6"/>
@@ -4310,7 +4286,7 @@
     <row r="25" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="32"/>
@@ -4376,7 +4352,7 @@
       <c r="B31" s="32"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E31" s="30"/>
       <c r="F31" s="6"/>
@@ -4433,7 +4409,7 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -4447,7 +4423,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -4461,7 +4437,7 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>

</xml_diff>